<commit_message>
remove completed status from xlsx
</commit_message>
<xml_diff>
--- a/client/public/assets/contactFormat.xlsx
+++ b/client/public/assets/contactFormat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\עבודה\טופס חקירות אפידמיולוגיות\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\עבודה\טופס חקירות אפידמיולוגיות\CoronaInvestigation\client\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E98EF1-0813-4927-8302-760DCAA17702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4E0C66-A645-4D16-AF7A-8607F6EA54C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="פריטים פעילים מסוג _פרטי מגעים_" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6397" uniqueCount="6374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6396" uniqueCount="6373">
   <si>
     <t>(אל תשנה) פרטי מגע</t>
   </si>
@@ -19133,9 +19133,6 @@
   </si>
   <si>
     <t>בטיפול</t>
-  </si>
-  <si>
-    <t>הושלם התחקור</t>
   </si>
   <si>
     <t>לא ניתן להשגה</t>
@@ -19841,10 +19838,10 @@
   <sheetPr codeName="dataSheet"/>
   <dimension ref="A1:AB755"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
+    <sheetView rightToLeft="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G280" sqref="G280"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -19929,7 +19926,7 @@
         <v>5</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>6373</v>
+        <v>6372</v>
       </c>
       <c r="R1" s="20" t="s">
         <v>29</v>
@@ -31344,7 +31341,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ערך רשימה" error="יש לבחור את הקמת דיווח בידוד‏‏ מהרשימה הנפתחת." promptTitle="קבוצת אפשרויות" prompt="‏‏בחר ערך מהרשימה הנפתחת." xr:uid="{007F4525-5D04-444D-9D07-7FE5B1837C7D}">
           <x14:formula1>
-            <xm:f>גיליון2!$A$1:$A$5</xm:f>
+            <xm:f>גיליון2!$A$1:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>Q2:Q335</xm:sqref>
         </x14:dataValidation>
@@ -31356,9 +31353,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B22D019-D9DA-4C03-90DB-EF4B33D7AABE}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -31385,11 +31382,6 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6371</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(ids): prevent duplicate ids (#740)
* move handle in finish investigation to
useTabManagement

* fix duplicate ids in ContactQuestioning tab

* check duplicatie ids on upload excel

* duplicate ids for interactions

* make the swal be above everything

* remove completed status from xlsx

* move setFormState to be after successful saving

* fix(duplicate-ids): code review syntax and design fix

* pr fixes

* fix(duplicate-ids): change for each to map and filter

* pr fixes

* fix(duplicate-ids): code review design errors in useDuplicateId

Co-authored-by: Elad Yashar <eladyashar1104@gmail.com@gmail.com>
</commit_message>
<xml_diff>
--- a/client/public/assets/contactFormat.xlsx
+++ b/client/public/assets/contactFormat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\עבודה\טופס חקירות אפידמיולוגיות\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\עבודה\טופס חקירות אפידמיולוגיות\CoronaInvestigation\client\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E98EF1-0813-4927-8302-760DCAA17702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4E0C66-A645-4D16-AF7A-8607F6EA54C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="פריטים פעילים מסוג _פרטי מגעים_" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6397" uniqueCount="6374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6396" uniqueCount="6373">
   <si>
     <t>(אל תשנה) פרטי מגע</t>
   </si>
@@ -19133,9 +19133,6 @@
   </si>
   <si>
     <t>בטיפול</t>
-  </si>
-  <si>
-    <t>הושלם התחקור</t>
   </si>
   <si>
     <t>לא ניתן להשגה</t>
@@ -19841,10 +19838,10 @@
   <sheetPr codeName="dataSheet"/>
   <dimension ref="A1:AB755"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
+    <sheetView rightToLeft="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G280" sqref="G280"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -19929,7 +19926,7 @@
         <v>5</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>6373</v>
+        <v>6372</v>
       </c>
       <c r="R1" s="20" t="s">
         <v>29</v>
@@ -31344,7 +31341,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ערך רשימה" error="יש לבחור את הקמת דיווח בידוד‏‏ מהרשימה הנפתחת." promptTitle="קבוצת אפשרויות" prompt="‏‏בחר ערך מהרשימה הנפתחת." xr:uid="{007F4525-5D04-444D-9D07-7FE5B1837C7D}">
           <x14:formula1>
-            <xm:f>גיליון2!$A$1:$A$5</xm:f>
+            <xm:f>גיליון2!$A$1:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>Q2:Q335</xm:sqref>
         </x14:dataValidation>
@@ -31356,9 +31353,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B22D019-D9DA-4C03-90DB-EF4B33D7AABE}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -31385,11 +31382,6 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6371</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(ids): duplicate ids dev (#753)
* move handle in finish investigation to
useTabManagement

* fix duplicate ids validation

* make the swal be above everything

* remove completed status from xlsx

* fix tests

* fix test 2

* fix test 3

* add another condition for
checking duplicate ids in the same event

* pr fixes
</commit_message>
<xml_diff>
--- a/client/public/assets/contactFormat.xlsx
+++ b/client/public/assets/contactFormat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\עבודה\טופס חקירות אפידמיולוגיות\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\עבודה\טופס חקירות אפידמיולוגיות\CoronaInvestigation\client\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E98EF1-0813-4927-8302-760DCAA17702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4E0C66-A645-4D16-AF7A-8607F6EA54C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="פריטים פעילים מסוג _פרטי מגעים_" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6397" uniqueCount="6374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6396" uniqueCount="6373">
   <si>
     <t>(אל תשנה) פרטי מגע</t>
   </si>
@@ -19133,9 +19133,6 @@
   </si>
   <si>
     <t>בטיפול</t>
-  </si>
-  <si>
-    <t>הושלם התחקור</t>
   </si>
   <si>
     <t>לא ניתן להשגה</t>
@@ -19841,10 +19838,10 @@
   <sheetPr codeName="dataSheet"/>
   <dimension ref="A1:AB755"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
+    <sheetView rightToLeft="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G280" sqref="G280"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -19929,7 +19926,7 @@
         <v>5</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>6373</v>
+        <v>6372</v>
       </c>
       <c r="R1" s="20" t="s">
         <v>29</v>
@@ -31344,7 +31341,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ערך רשימה" error="יש לבחור את הקמת דיווח בידוד‏‏ מהרשימה הנפתחת." promptTitle="קבוצת אפשרויות" prompt="‏‏בחר ערך מהרשימה הנפתחת." xr:uid="{007F4525-5D04-444D-9D07-7FE5B1837C7D}">
           <x14:formula1>
-            <xm:f>גיליון2!$A$1:$A$5</xm:f>
+            <xm:f>גיליון2!$A$1:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>Q2:Q335</xm:sqref>
         </x14:dataValidation>
@@ -31356,9 +31353,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B22D019-D9DA-4C03-90DB-EF4B33D7AABE}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -31385,11 +31382,6 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6371</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(): removed geriatrics from work options
</commit_message>
<xml_diff>
--- a/client/public/assets/contactFormat.xlsx
+++ b/client/public/assets/contactFormat.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\עבודה\טופס חקירות אפידמיולוגיות\CoronaInvestigation\client\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4E0C66-A645-4D16-AF7A-8607F6EA54C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A8B38E-0D24-4552-A502-5F3F0FDF6210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="פריטים פעילים מסוג _פרטי מגעים_" sheetId="1" r:id="rId1"/>
-    <sheet name="גיליון2" sheetId="4" r:id="rId2"/>
-    <sheet name="גיליון1" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="hiddenSheet" sheetId="2" state="veryHidden" r:id="rId4"/>
+    <sheet name="גיליון3" sheetId="5" state="hidden" r:id="rId2"/>
+    <sheet name="גיליון2" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="גיליון1" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="hiddenSheet" sheetId="2" state="veryHidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6396" uniqueCount="6373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6404" uniqueCount="6374">
   <si>
     <t>(אל תשנה) פרטי מגע</t>
   </si>
@@ -19142,6 +19143,9 @@
   </si>
   <si>
     <t>סטטוס</t>
+  </si>
+  <si>
+    <t>משרד ממשלתי או רשות מקומית</t>
   </si>
 </sst>
 </file>
@@ -19181,11 +19185,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -19838,10 +19844,10 @@
   <sheetPr codeName="dataSheet"/>
   <dimension ref="A1:AB755"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomLeft" activeCell="W2" sqref="W1:W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -19977,7 +19983,7 @@
       <c r="T2" s="25"/>
       <c r="U2" s="25"/>
       <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
+      <c r="W2" s="32"/>
       <c r="X2" s="30"/>
       <c r="Y2"/>
       <c r="Z2"/>
@@ -31296,7 +31302,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="130" yWindow="430" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="130" yWindow="430" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ערך רשימה" error="יש לבחור את הקמת דיווח בידוד‏‏ מהרשימה הנפתחת." promptTitle="קבוצת אפשרויות" prompt="‏‏בחר ערך מהרשימה הנפתחת." xr:uid="{00000000-0002-0000-0000-000010000000}">
           <x14:formula1>
             <xm:f>hiddenSheet!$A$3:$A$3</xm:f>
@@ -31337,13 +31343,19 @@
           <x14:formula1>
             <xm:f>hiddenSheet!$A$9:$I$9</xm:f>
           </x14:formula1>
-          <xm:sqref>AB336:AB1048576 W2:W335</xm:sqref>
+          <xm:sqref>AB336:AB1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ערך רשימה" error="יש לבחור את הקמת דיווח בידוד‏‏ מהרשימה הנפתחת." promptTitle="קבוצת אפשרויות" prompt="‏‏בחר ערך מהרשימה הנפתחת." xr:uid="{007F4525-5D04-444D-9D07-7FE5B1837C7D}">
           <x14:formula1>
             <xm:f>גיליון2!$A$1:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>Q2:Q335</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ערך רשימה" error="יש לבחור את תחום עיסוק‏‏ מהרשימה הנפתחת." promptTitle="קבוצת אפשרויות" prompt="‏‏בחר ערך מהרשימה הנפתחת." xr:uid="{B841C271-2062-4511-AF11-174114CF33E2}">
+          <x14:formula1>
+            <xm:f>גיליון3!$A$1:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>W2:W335</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -31352,10 +31364,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8255248-ED6A-4F65-8CBB-EFC59D211349}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>6373</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B22D019-D9DA-4C03-90DB-EF4B33D7AABE}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -31389,7 +31456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1586"/>
   <sheetViews>
@@ -63144,7 +63211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="hiddenDataSheet"/>
   <dimension ref="A1:I9"/>

</xml_diff>

<commit_message>
fix(): removed geriatrics from work options (#762)
Co-authored-by: EmilyLip <mily7975@gmail.com>
</commit_message>
<xml_diff>
--- a/client/public/assets/contactFormat.xlsx
+++ b/client/public/assets/contactFormat.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\עבודה\טופס חקירות אפידמיולוגיות\CoronaInvestigation\client\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4E0C66-A645-4D16-AF7A-8607F6EA54C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A8B38E-0D24-4552-A502-5F3F0FDF6210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="פריטים פעילים מסוג _פרטי מגעים_" sheetId="1" r:id="rId1"/>
-    <sheet name="גיליון2" sheetId="4" r:id="rId2"/>
-    <sheet name="גיליון1" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="hiddenSheet" sheetId="2" state="veryHidden" r:id="rId4"/>
+    <sheet name="גיליון3" sheetId="5" state="hidden" r:id="rId2"/>
+    <sheet name="גיליון2" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="גיליון1" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="hiddenSheet" sheetId="2" state="veryHidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6396" uniqueCount="6373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6404" uniqueCount="6374">
   <si>
     <t>(אל תשנה) פרטי מגע</t>
   </si>
@@ -19142,6 +19143,9 @@
   </si>
   <si>
     <t>סטטוס</t>
+  </si>
+  <si>
+    <t>משרד ממשלתי או רשות מקומית</t>
   </si>
 </sst>
 </file>
@@ -19181,11 +19185,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -19838,10 +19844,10 @@
   <sheetPr codeName="dataSheet"/>
   <dimension ref="A1:AB755"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomLeft" activeCell="W2" sqref="W1:W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -19977,7 +19983,7 @@
       <c r="T2" s="25"/>
       <c r="U2" s="25"/>
       <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
+      <c r="W2" s="32"/>
       <c r="X2" s="30"/>
       <c r="Y2"/>
       <c r="Z2"/>
@@ -31296,7 +31302,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="130" yWindow="430" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="130" yWindow="430" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ערך רשימה" error="יש לבחור את הקמת דיווח בידוד‏‏ מהרשימה הנפתחת." promptTitle="קבוצת אפשרויות" prompt="‏‏בחר ערך מהרשימה הנפתחת." xr:uid="{00000000-0002-0000-0000-000010000000}">
           <x14:formula1>
             <xm:f>hiddenSheet!$A$3:$A$3</xm:f>
@@ -31337,13 +31343,19 @@
           <x14:formula1>
             <xm:f>hiddenSheet!$A$9:$I$9</xm:f>
           </x14:formula1>
-          <xm:sqref>AB336:AB1048576 W2:W335</xm:sqref>
+          <xm:sqref>AB336:AB1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ערך רשימה" error="יש לבחור את הקמת דיווח בידוד‏‏ מהרשימה הנפתחת." promptTitle="קבוצת אפשרויות" prompt="‏‏בחר ערך מהרשימה הנפתחת." xr:uid="{007F4525-5D04-444D-9D07-7FE5B1837C7D}">
           <x14:formula1>
             <xm:f>גיליון2!$A$1:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>Q2:Q335</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ערך רשימה" error="יש לבחור את תחום עיסוק‏‏ מהרשימה הנפתחת." promptTitle="קבוצת אפשרויות" prompt="‏‏בחר ערך מהרשימה הנפתחת." xr:uid="{B841C271-2062-4511-AF11-174114CF33E2}">
+          <x14:formula1>
+            <xm:f>גיליון3!$A$1:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>W2:W335</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -31352,10 +31364,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8255248-ED6A-4F65-8CBB-EFC59D211349}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>6373</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B22D019-D9DA-4C03-90DB-EF4B33D7AABE}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -31389,7 +31456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1586"/>
   <sheetViews>
@@ -63144,7 +63211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="hiddenDataSheet"/>
   <dimension ref="A1:I9"/>

</xml_diff>